<commit_message>
Calculation of initial stress anisotropy was improved
</commit_message>
<xml_diff>
--- a/TunnelFaceAdvRate.xlsx
+++ b/TunnelFaceAdvRate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lflessati\surfdrive - Luca Flessati@surfdrive.surf.nl\MonA\TunnelFace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F87FD1-FBA8-47AF-B878-8553A589AD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0722552-26B8-48E2-A28D-01693944588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Input</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Position of water table w.r.t. tunnel axis</t>
   </si>
   <si>
-    <t>u</t>
-  </si>
-  <si>
     <t>sf'0</t>
   </si>
   <si>
@@ -364,13 +361,23 @@
   <si>
     <t>(kN)</t>
   </si>
+  <si>
+    <t>u0</t>
+  </si>
+  <si>
+    <t>sv0</t>
+  </si>
+  <si>
+    <t>Average total vertical stress at the tunnel face</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -428,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -438,6 +445,8 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,10 +586,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.02847</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.05</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.1000000000000001</c:v>
@@ -589,7 +598,7 @@
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="88" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1804,7 +1813,7 @@
       </c>
       <c r="K4" s="3">
         <f>+B47*B44*B28/B20</f>
-        <v>0.50435478752053409</v>
+        <v>0.64183098824903528</v>
       </c>
       <c r="L4" t="s">
         <v>4</v>
@@ -1818,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1827,17 +1836,17 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="10">
+        <f>PI()*B4^2/4*(B16+K4)*B7</f>
+        <v>2578.9820855596195</v>
+      </c>
+      <c r="L5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" t="s">
         <v>83</v>
-      </c>
-      <c r="K5" s="8">
-        <f>PI()*B4^2/4*(B16+K4)*B7</f>
-        <v>2363.0349744335722</v>
-      </c>
-      <c r="L5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1845,7 +1854,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1854,17 +1863,17 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" s="8">
         <f>K4/(1.5*B4)*100</f>
-        <v>3.3623652501368935</v>
+        <v>4.2788732549935684</v>
       </c>
       <c r="L6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1964,35 +1973,35 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="6">
         <v>1E-4</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -2001,7 +2010,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2009,13 +2018,28 @@
         <v>26</v>
       </c>
     </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19">
+        <f>B7*B5</f>
+        <v>1800</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20">
-        <f>+B30*B7*(B5)</f>
-        <v>1560</v>
+        <f>B21+B22</f>
+        <v>1800</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -2026,11 +2050,11 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B21">
         <f>B6*B8</f>
-        <v>780</v>
+        <v>850</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2041,98 +2065,98 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
-        <f>B20-B21</f>
-        <v>780</v>
+        <f>B23*B12</f>
+        <v>950</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23">
-        <f>B22/B12</f>
-        <v>780</v>
+        <f>B19-B21</f>
+        <v>950</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <f>(B23+2*B22)/3</f>
-        <v>780</v>
+        <v>950</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <f>6*SIN(RADIANS(B11))/(3+SIN(RADIANS(B11)))</f>
         <v>0.74086835765159731</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <f>B25/2*B24</f>
-        <v>288.93865948412292</v>
+        <v>351.91246988450871</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27">
-        <f>0.0006*B11^2-0.01*B11+1</f>
-        <v>1.125</v>
+        <v>53</v>
+      </c>
+      <c r="B27" s="9">
+        <f>0.0005*B11^2-0.009*B11+1</f>
+        <v>1.0874999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2">
         <f>B26*B27</f>
-        <v>325.0559919196383</v>
+        <v>382.70481099940321</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2140,7 +2164,7 @@
         <v>14</v>
       </c>
       <c r="B30">
-        <f>+(B12*(B7-9.81)+9.81)/B7</f>
+        <f>B20/B19</f>
         <v>1</v>
       </c>
       <c r="D30" t="s">
@@ -2158,7 +2182,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32">
         <f>(B7-B8)*B4*(1/(9*TAN(RADIANS(B11)))-0.05)</f>
@@ -2168,12 +2192,12 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <f>+B9/(3*(1-2*B10))</f>
@@ -2183,7 +2207,7 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2198,67 +2222,67 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36">
         <f>1.5*B4/B14</f>
         <v>1.5</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5">
         <f>B8*B4^2/(B15*B34*B36)</f>
         <v>320.00000000000006</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="5">
         <f>0.725+(1-0.725)*(0.065*B37^0.635)/(0.065*B37^0.635+1)</f>
         <v>0.92216868770563898</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="5">
         <f>0.686+(B31-0.686)*(0.2*B37^0.635)/(0.2*B37^0.635+1)</f>
         <v>1.4641673146201444</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="5">
         <f>(B22-B32)/B28+1.6*B37</f>
-        <v>514.34166471084734</v>
+        <v>514.43313415082514</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2267,7 +2291,7 @@
       </c>
       <c r="B44">
         <f>1/3*B20*B4/B35</f>
-        <v>0.18026666666666669</v>
+        <v>0.20800000000000002</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -2282,7 +2306,7 @@
       </c>
       <c r="B45">
         <f>+(B20-B13)/B28</f>
-        <v>4.7991731848637009</v>
+        <v>4.7033639198301245</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2290,8 +2314,8 @@
         <v>19</v>
       </c>
       <c r="B47">
-        <f>+IF(B45&lt;B40,B45/B39,B31/B39*EXP(B45/B31-1)+(B45-B40)/(B41-B45))</f>
-        <v>13.427252063199944</v>
+        <f>+IF(B45&lt;B40,B45/B39,B40/B39*EXP(B45/B40-1)+(B45-B40)/(B41-B45))</f>
+        <v>14.513291888266467</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -2299,7 +2323,7 @@
         <v>20</v>
       </c>
       <c r="C50">
-        <v>1.02847</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -2307,7 +2331,7 @@
         <v>22.5</v>
       </c>
       <c r="C51">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -2331,12 +2355,12 @@
         <v>30</v>
       </c>
       <c r="C54">
-        <v>1.2</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="66" spans="11:11">
       <c r="K66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>